<commit_message>
update imports, models, migrations, seeders, and users.xlsx
</commit_message>
<xml_diff>
--- a/database/seeders/data/users.xlsx
+++ b/database/seeders/data/users.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\syaukaniabr\projects\laravel\djpb-inzil-app\database\seeders\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD064E76-81DA-4AFF-9860-64678A0B86D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E450C4-DD84-4F1A-82E4-96E0CE0864C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="219">
   <si>
     <t>Nama</t>
   </si>
@@ -693,13 +693,19 @@
   </si>
   <si>
     <t>Photo Profile</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>+6282149095841</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -845,6 +851,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1192,7 +1204,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1201,6 +1213,7 @@
     </xf>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="42" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1247,7 +1260,11 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1290,8 +1307,8 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="query" backgroundRefresh="0" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="10" unboundColumnsRight="1">
-    <queryTableFields count="7">
+  <queryTableRefresh nextId="11" unboundColumnsRight="2">
+    <queryTableFields count="8">
       <queryTableField id="1" name="Nama" tableColumnId="1"/>
       <queryTableField id="6" name="Email" tableColumnId="2"/>
       <queryTableField id="2" name="NIP" tableColumnId="3"/>
@@ -1299,6 +1316,7 @@
       <queryTableField id="4" name="BagianBidang" tableColumnId="5"/>
       <queryTableField id="5" name="Tanggal Lahir" tableColumnId="6"/>
       <queryTableField id="9" dataBound="0" tableColumnId="7"/>
+      <queryTableField id="10" dataBound="0" tableColumnId="8"/>
     </queryTableFields>
     <queryTableDeletedFields count="2">
       <deletedField name="Item Type"/>
@@ -1309,16 +1327,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_query" displayName="Table_query" ref="A1:G43" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:G43" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="Title" name="Nama" queryTableFieldId="1" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="Email" name="Email" queryTableFieldId="6" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="NIP" name="NIP" queryTableFieldId="2" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" uniqueName="Jabatan" name="Jabatan" queryTableFieldId="3" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" uniqueName="UnitKerja" name="BagianBidang" queryTableFieldId="4" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="TanggalLahir" name="Tanggal Lahir" queryTableFieldId="5" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{B5566D31-C0DE-4975-950B-428896D6ABF1}" uniqueName="7" name="Photo Profile" queryTableFieldId="9" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_query" displayName="Table_query" ref="A1:H43" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:H43" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="Title" name="Nama" queryTableFieldId="1" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="Email" name="Email" queryTableFieldId="6" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="NIP" name="NIP" queryTableFieldId="2" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" uniqueName="Jabatan" name="Jabatan" queryTableFieldId="3" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" uniqueName="UnitKerja" name="BagianBidang" queryTableFieldId="4" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="TanggalLahir" name="Tanggal Lahir" queryTableFieldId="5" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{B5566D31-C0DE-4975-950B-428896D6ABF1}" uniqueName="7" name="Photo Profile" queryTableFieldId="9" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{9A6D1AE2-37D4-4834-A56A-25340331BFC0}" uniqueName="8" name="Phone" queryTableFieldId="10" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1623,8 +1642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1664,6 +1683,9 @@
       <c r="G1" t="s">
         <v>216</v>
       </c>
+      <c r="H1" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -1687,6 +1709,7 @@
       <c r="G2" s="5" t="s">
         <v>181</v>
       </c>
+      <c r="H2" s="6"/>
       <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -1711,6 +1734,9 @@
       <c r="G3" s="1" t="s">
         <v>194</v>
       </c>
+      <c r="H3" s="6" t="s">
+        <v>218</v>
+      </c>
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -1735,6 +1761,7 @@
       <c r="G4" s="1" t="s">
         <v>174</v>
       </c>
+      <c r="H4" s="6"/>
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -1759,6 +1786,7 @@
       <c r="G5" s="1" t="s">
         <v>182</v>
       </c>
+      <c r="H5" s="6"/>
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -1783,6 +1811,7 @@
       <c r="G6" s="1" t="s">
         <v>175</v>
       </c>
+      <c r="H6" s="6"/>
       <c r="I6" s="2"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -1807,6 +1836,7 @@
       <c r="G7" s="1" t="s">
         <v>197</v>
       </c>
+      <c r="H7" s="6"/>
       <c r="I7" s="2"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -1831,6 +1861,7 @@
       <c r="G8" s="1" t="s">
         <v>176</v>
       </c>
+      <c r="H8" s="6"/>
       <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -1855,6 +1886,7 @@
       <c r="G9" s="1" t="s">
         <v>177</v>
       </c>
+      <c r="H9" s="6"/>
       <c r="I9" s="2"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -1879,6 +1911,7 @@
       <c r="G10" s="1" t="s">
         <v>183</v>
       </c>
+      <c r="H10" s="6"/>
       <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -1903,6 +1936,7 @@
       <c r="G11" s="1" t="s">
         <v>215</v>
       </c>
+      <c r="H11" s="6"/>
       <c r="I11" s="2"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -1927,6 +1961,7 @@
       <c r="G12" s="1" t="s">
         <v>184</v>
       </c>
+      <c r="H12" s="6"/>
       <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -1951,6 +1986,7 @@
       <c r="G13" s="1" t="s">
         <v>178</v>
       </c>
+      <c r="H13" s="6"/>
       <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -1975,6 +2011,7 @@
       <c r="G14" s="1" t="s">
         <v>185</v>
       </c>
+      <c r="H14" s="6"/>
       <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -1999,6 +2036,7 @@
       <c r="G15" s="1" t="s">
         <v>186</v>
       </c>
+      <c r="H15" s="6"/>
       <c r="I15" s="2"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -2023,6 +2061,7 @@
       <c r="G16" s="1" t="s">
         <v>195</v>
       </c>
+      <c r="H16" s="6"/>
       <c r="I16" s="2"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
@@ -2047,6 +2086,7 @@
       <c r="G17" s="1" t="s">
         <v>179</v>
       </c>
+      <c r="H17" s="6"/>
       <c r="I17" s="2"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
@@ -2071,6 +2111,7 @@
       <c r="G18" s="1" t="s">
         <v>187</v>
       </c>
+      <c r="H18" s="6"/>
       <c r="I18" s="2"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
@@ -2095,6 +2136,7 @@
       <c r="G19" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="H19" s="6"/>
       <c r="I19" s="2"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
@@ -2119,6 +2161,7 @@
       <c r="G20" s="1" t="s">
         <v>196</v>
       </c>
+      <c r="H20" s="6"/>
       <c r="I20" s="2"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
@@ -2143,6 +2186,7 @@
       <c r="G21" s="1" t="s">
         <v>189</v>
       </c>
+      <c r="H21" s="6"/>
       <c r="I21" s="2"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
@@ -2167,6 +2211,7 @@
       <c r="G22" s="1" t="s">
         <v>190</v>
       </c>
+      <c r="H22" s="6"/>
       <c r="I22" s="2"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
@@ -2191,6 +2236,7 @@
       <c r="G23" s="1" t="s">
         <v>191</v>
       </c>
+      <c r="H23" s="6"/>
       <c r="I23" s="2"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
@@ -2215,6 +2261,7 @@
       <c r="G24" s="1" t="s">
         <v>180</v>
       </c>
+      <c r="H24" s="6"/>
       <c r="I24" s="2"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
@@ -2239,6 +2286,7 @@
       <c r="G25" s="1" t="s">
         <v>192</v>
       </c>
+      <c r="H25" s="6"/>
       <c r="I25" s="2"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
@@ -2263,6 +2311,7 @@
       <c r="G26" s="1" t="s">
         <v>193</v>
       </c>
+      <c r="H26" s="6"/>
       <c r="I26" s="2"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
@@ -2287,6 +2336,7 @@
       <c r="G27" s="1" t="s">
         <v>198</v>
       </c>
+      <c r="H27" s="6"/>
       <c r="I27" s="2"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
@@ -2311,6 +2361,7 @@
       <c r="G28" s="1" t="s">
         <v>199</v>
       </c>
+      <c r="H28" s="6"/>
       <c r="I28" s="2"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
@@ -2335,6 +2386,7 @@
       <c r="G29" s="1" t="s">
         <v>200</v>
       </c>
+      <c r="H29" s="6"/>
       <c r="I29" s="2"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
@@ -2359,6 +2411,7 @@
       <c r="G30" s="1" t="s">
         <v>201</v>
       </c>
+      <c r="H30" s="6"/>
       <c r="I30" s="2"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
@@ -2383,6 +2436,7 @@
       <c r="G31" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="H31" s="6"/>
       <c r="I31" s="2"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
@@ -2407,6 +2461,7 @@
       <c r="G32" s="1" t="s">
         <v>203</v>
       </c>
+      <c r="H32" s="6"/>
       <c r="I32" s="2"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
@@ -2431,6 +2486,7 @@
       <c r="G33" s="1" t="s">
         <v>204</v>
       </c>
+      <c r="H33" s="6"/>
       <c r="I33" s="2"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
@@ -2455,6 +2511,7 @@
       <c r="G34" s="1" t="s">
         <v>205</v>
       </c>
+      <c r="H34" s="6"/>
       <c r="I34" s="2"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
@@ -2479,6 +2536,7 @@
       <c r="G35" s="1" t="s">
         <v>206</v>
       </c>
+      <c r="H35" s="6"/>
       <c r="I35" s="2"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
@@ -2503,6 +2561,7 @@
       <c r="G36" s="1" t="s">
         <v>207</v>
       </c>
+      <c r="H36" s="6"/>
       <c r="I36" s="2"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
@@ -2527,6 +2586,7 @@
       <c r="G37" s="1" t="s">
         <v>208</v>
       </c>
+      <c r="H37" s="6"/>
       <c r="I37" s="2"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
@@ -2551,6 +2611,7 @@
       <c r="G38" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="H38" s="6"/>
       <c r="I38" s="2"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
@@ -2575,6 +2636,7 @@
       <c r="G39" s="1" t="s">
         <v>210</v>
       </c>
+      <c r="H39" s="6"/>
       <c r="I39" s="2"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
@@ -2599,6 +2661,7 @@
       <c r="G40" s="1" t="s">
         <v>211</v>
       </c>
+      <c r="H40" s="6"/>
       <c r="I40" s="2"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
@@ -2623,6 +2686,7 @@
       <c r="G41" s="1" t="s">
         <v>212</v>
       </c>
+      <c r="H41" s="6"/>
       <c r="I41" s="2"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
@@ -2647,6 +2711,7 @@
       <c r="G42" s="1" t="s">
         <v>213</v>
       </c>
+      <c r="H42" s="6"/>
       <c r="I42" s="2"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
@@ -2671,9 +2736,11 @@
       <c r="G43" s="1" t="s">
         <v>214</v>
       </c>
+      <c r="H43" s="6"/>
       <c r="I43" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="20" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{7329C114-D6EB-4909-9C57-4ABFC70E59F1}"/>
     <hyperlink ref="B6" r:id="rId2" xr:uid="{A582FE80-2D0D-41B7-9FE0-03F6FE0D5C02}"/>

</xml_diff>